<commit_message>
Update Bug Reporter sub app
</commit_message>
<xml_diff>
--- a/lang/words_dict.xlsx
+++ b/lang/words_dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\si lab\Matlab Projects\Registration\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F98F0C8-F86D-4B9F-965A-EAE6DB93CFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD645DF-6BB4-41E0-B23B-8F4C0AC1B3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1020" windowWidth="29010" windowHeight="14265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2262" uniqueCount="2248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2268" uniqueCount="2254">
   <si>
     <t>文件</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -7074,10 +7074,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>问题报告程序不会收集您的隐私</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>此处包含用于复现问题的附加文件</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -7105,10 +7101,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>The problem reporting process does not collect your privacy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Attach Folder</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -7173,9 +7165,6 @@
     <t>Процедура сообщения о проблеме:</t>
   </si>
   <si>
-    <t>Процесс сообщения о проблемах не обеспечивает конфиденциальность вашей информации.</t>
-  </si>
-  <si>
     <t>Дополнительные файлы для воспроизведения проблемы включены здесь.</t>
   </si>
   <si>
@@ -7206,9 +7195,6 @@
     <t>Procédure de signalement des problèmes :</t>
   </si>
   <si>
-    <t>Le processus de signalement de problèmes ne collecte pas votre vie privée</t>
-  </si>
-  <si>
     <t>Des fichiers supplémentaires pour reproduire le problème sont inclus ici</t>
   </si>
   <si>
@@ -7245,9 +7231,6 @@
     <t>Procedimiento de notificación de problemas:</t>
   </si>
   <si>
-    <t>El proceso de notificación de problemas no recopila su privacidad</t>
-  </si>
-  <si>
     <t>Aquí se incluyen archivos adicionales para reproducir el problema.</t>
   </si>
   <si>
@@ -7733,6 +7716,46 @@
   </si>
   <si>
     <t>Continuar</t>
+  </si>
+  <si>
+    <t>问题报告程序不会收集您的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>隐私</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>privacy</t>
+  </si>
+  <si>
+    <t>PRIVACY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>confidentialité</t>
+  </si>
+  <si>
+    <t>privacidad</t>
+  </si>
+  <si>
+    <t>конфиденциальность</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The problem reporting process does not collect your </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Процесс сообщения о проблемах не собирает ваши </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Le processus de signalement de problèmes ne collecte pas vos </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">El proceso de informe de problemas no recopila su </t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -8066,10 +8089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F377"/>
+  <dimension ref="A1:F378"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="E91" sqref="E91"/>
+    <sheetView tabSelected="1" topLeftCell="C348" workbookViewId="0">
+      <selection activeCell="F369" sqref="F369"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -8607,24 +8630,24 @@
         <v>1476</v>
       </c>
       <c r="B27" t="s">
+        <v>2129</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2130</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2132</v>
+      </c>
+      <c r="E27" t="s">
+        <v>2133</v>
+      </c>
+      <c r="F27" t="s">
         <v>2134</v>
-      </c>
-      <c r="C27" t="s">
-        <v>2135</v>
-      </c>
-      <c r="D27" t="s">
-        <v>2137</v>
-      </c>
-      <c r="E27" t="s">
-        <v>2138</v>
-      </c>
-      <c r="F27" t="s">
-        <v>2139</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>2136</v>
+        <v>2131</v>
       </c>
       <c r="B28" t="s">
         <v>15</v>
@@ -9784,7 +9807,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>2169</v>
+        <v>2164</v>
       </c>
       <c r="B86" t="s">
         <v>72</v>
@@ -9984,22 +10007,22 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>2243</v>
+        <v>2238</v>
       </c>
       <c r="B96" t="s">
+        <v>2237</v>
+      </c>
+      <c r="C96" t="s">
+        <v>2239</v>
+      </c>
+      <c r="D96" t="s">
+        <v>2240</v>
+      </c>
+      <c r="E96" t="s">
+        <v>2241</v>
+      </c>
+      <c r="F96" t="s">
         <v>2242</v>
-      </c>
-      <c r="C96" t="s">
-        <v>2244</v>
-      </c>
-      <c r="D96" t="s">
-        <v>2245</v>
-      </c>
-      <c r="E96" t="s">
-        <v>2246</v>
-      </c>
-      <c r="F96" t="s">
-        <v>2247</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
@@ -10084,7 +10107,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>2131</v>
+        <v>2126</v>
       </c>
       <c r="B101" t="s">
         <v>82</v>
@@ -10244,7 +10267,7 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>2132</v>
+        <v>2127</v>
       </c>
       <c r="B109" t="s">
         <v>86</v>
@@ -10524,7 +10547,7 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>2133</v>
+        <v>2128</v>
       </c>
       <c r="B123" t="s">
         <v>98</v>
@@ -10804,7 +10827,7 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>2140</v>
+        <v>2135</v>
       </c>
       <c r="B137" t="s">
         <v>112</v>
@@ -10884,7 +10907,7 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>2141</v>
+        <v>2136</v>
       </c>
       <c r="B141" t="s">
         <v>116</v>
@@ -11024,7 +11047,7 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>2166</v>
+        <v>2161</v>
       </c>
       <c r="B148" t="s">
         <v>123</v>
@@ -11444,7 +11467,7 @@
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>2167</v>
+        <v>2162</v>
       </c>
       <c r="B169" t="s">
         <v>142</v>
@@ -12264,7 +12287,7 @@
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>2168</v>
+        <v>2163</v>
       </c>
       <c r="B210" t="s">
         <v>163</v>
@@ -15004,621 +15027,641 @@
     </row>
     <row r="347" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
-        <v>2113</v>
+        <v>2108</v>
       </c>
       <c r="B347" t="s">
         <v>2047</v>
       </c>
       <c r="C347" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="D347" t="s">
-        <v>2075</v>
+        <v>2073</v>
       </c>
       <c r="E347" t="s">
-        <v>2088</v>
+        <v>2085</v>
       </c>
       <c r="F347" t="s">
-        <v>2099</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="348" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
-        <v>2112</v>
+        <v>2107</v>
       </c>
       <c r="B348" t="s">
         <v>2048</v>
       </c>
       <c r="C348" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
       <c r="D348" t="s">
-        <v>2076</v>
+        <v>2074</v>
       </c>
       <c r="E348" t="s">
-        <v>2089</v>
+        <v>2086</v>
       </c>
       <c r="F348" t="s">
-        <v>2100</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="349" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
-        <v>2114</v>
+        <v>2109</v>
       </c>
       <c r="B349" t="s">
         <v>2050</v>
       </c>
       <c r="C349" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
       <c r="D349" t="s">
-        <v>2077</v>
+        <v>2075</v>
       </c>
       <c r="E349" t="s">
-        <v>2090</v>
+        <v>2087</v>
       </c>
       <c r="F349" t="s">
-        <v>2101</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="350" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
-        <v>2115</v>
+        <v>2110</v>
       </c>
       <c r="B350" t="s">
         <v>2051</v>
       </c>
       <c r="C350" t="s">
-        <v>2068</v>
+        <v>2066</v>
       </c>
       <c r="D350" t="s">
-        <v>2078</v>
+        <v>2076</v>
       </c>
       <c r="E350" t="s">
-        <v>2067</v>
+        <v>2065</v>
       </c>
       <c r="F350" t="s">
-        <v>2102</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="351" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
-        <v>2116</v>
+        <v>2111</v>
       </c>
       <c r="B351" t="s">
         <v>2052</v>
       </c>
       <c r="C351" t="s">
-        <v>2069</v>
+        <v>2067</v>
       </c>
       <c r="D351" t="s">
-        <v>2079</v>
+        <v>2077</v>
       </c>
       <c r="E351" t="s">
-        <v>2091</v>
+        <v>2088</v>
       </c>
       <c r="F351" t="s">
-        <v>2103</v>
+        <v>2099</v>
       </c>
     </row>
     <row r="352" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
-        <v>2117</v>
+        <v>2112</v>
       </c>
       <c r="B352" t="s">
         <v>2053</v>
       </c>
       <c r="C352" t="s">
-        <v>2071</v>
+        <v>2069</v>
       </c>
       <c r="D352" t="s">
-        <v>2080</v>
+        <v>2078</v>
       </c>
       <c r="E352" t="s">
-        <v>2070</v>
+        <v>2068</v>
       </c>
       <c r="F352" t="s">
-        <v>2104</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="353" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
-        <v>2171</v>
+        <v>2166</v>
       </c>
       <c r="B353" t="s">
+        <v>2165</v>
+      </c>
+      <c r="C353" t="s">
+        <v>2167</v>
+      </c>
+      <c r="D353" t="s">
+        <v>2168</v>
+      </c>
+      <c r="E353" t="s">
+        <v>2169</v>
+      </c>
+      <c r="F353" t="s">
         <v>2170</v>
-      </c>
-      <c r="C353" t="s">
-        <v>2172</v>
-      </c>
-      <c r="D353" t="s">
-        <v>2173</v>
-      </c>
-      <c r="E353" t="s">
-        <v>2174</v>
-      </c>
-      <c r="F353" t="s">
-        <v>2175</v>
       </c>
     </row>
     <row r="354" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
-        <v>2118</v>
+        <v>2113</v>
       </c>
       <c r="B354" t="s">
         <v>2054</v>
       </c>
       <c r="C354" t="s">
-        <v>2072</v>
+        <v>2070</v>
       </c>
       <c r="D354" t="s">
-        <v>2081</v>
+        <v>2079</v>
       </c>
       <c r="E354" t="s">
-        <v>2092</v>
+        <v>2089</v>
       </c>
       <c r="F354" t="s">
-        <v>2105</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="355" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
-        <v>2119</v>
+        <v>2114</v>
       </c>
       <c r="B355" t="s">
         <v>2055</v>
       </c>
       <c r="C355" t="s">
-        <v>2073</v>
+        <v>2071</v>
       </c>
       <c r="D355" t="s">
-        <v>2082</v>
+        <v>2080</v>
       </c>
       <c r="E355" t="s">
-        <v>2093</v>
+        <v>2090</v>
       </c>
       <c r="F355" t="s">
-        <v>2106</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="356" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
-        <v>2120</v>
+        <v>2115</v>
       </c>
       <c r="B356" t="s">
         <v>2056</v>
       </c>
       <c r="C356" t="s">
-        <v>2074</v>
+        <v>2072</v>
       </c>
       <c r="D356" t="s">
-        <v>2083</v>
+        <v>2081</v>
       </c>
       <c r="E356" t="s">
-        <v>2094</v>
+        <v>2091</v>
       </c>
       <c r="F356" t="s">
-        <v>2107</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="357" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
-        <v>2121</v>
+        <v>2116</v>
       </c>
       <c r="B357" t="s">
+        <v>2062</v>
+      </c>
+      <c r="C357" t="s">
         <v>2063</v>
       </c>
-      <c r="C357" t="s">
-        <v>2064</v>
-      </c>
       <c r="D357" t="s">
-        <v>2084</v>
+        <v>2082</v>
       </c>
       <c r="E357" t="s">
-        <v>2095</v>
+        <v>2092</v>
       </c>
       <c r="F357" t="s">
-        <v>2108</v>
+        <v>2104</v>
       </c>
     </row>
     <row r="358" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
-        <v>2122</v>
+        <v>2117</v>
       </c>
       <c r="B358" t="s">
-        <v>2057</v>
+        <v>2243</v>
       </c>
       <c r="C358" t="s">
-        <v>2065</v>
+        <v>2250</v>
       </c>
       <c r="D358" t="s">
-        <v>2085</v>
+        <v>2251</v>
       </c>
       <c r="E358" t="s">
-        <v>2096</v>
+        <v>2252</v>
       </c>
       <c r="F358" t="s">
-        <v>2109</v>
+        <v>2253</v>
       </c>
     </row>
     <row r="359" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
-        <v>2123</v>
+        <v>2246</v>
       </c>
       <c r="B359" t="s">
-        <v>2058</v>
+        <v>2244</v>
       </c>
       <c r="C359" t="s">
-        <v>2059</v>
+        <v>2245</v>
       </c>
       <c r="D359" t="s">
-        <v>2086</v>
+        <v>2249</v>
       </c>
       <c r="E359" t="s">
-        <v>2097</v>
+        <v>2247</v>
       </c>
       <c r="F359" t="s">
-        <v>2110</v>
+        <v>2248</v>
       </c>
     </row>
     <row r="360" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
-        <v>2177</v>
+        <v>2118</v>
       </c>
       <c r="B360" t="s">
-        <v>2176</v>
+        <v>2057</v>
       </c>
       <c r="C360" t="s">
-        <v>2178</v>
+        <v>2058</v>
       </c>
       <c r="D360" t="s">
-        <v>2179</v>
+        <v>2083</v>
       </c>
       <c r="E360" t="s">
-        <v>2180</v>
+        <v>2093</v>
       </c>
       <c r="F360" t="s">
-        <v>2181</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="361" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
-        <v>2207</v>
+        <v>2172</v>
       </c>
       <c r="B361" t="s">
-        <v>2206</v>
+        <v>2171</v>
       </c>
       <c r="C361" t="s">
-        <v>2208</v>
+        <v>2173</v>
       </c>
       <c r="D361" t="s">
-        <v>2209</v>
+        <v>2174</v>
       </c>
       <c r="E361" t="s">
-        <v>2210</v>
+        <v>2175</v>
       </c>
       <c r="F361" t="s">
-        <v>2211</v>
+        <v>2176</v>
       </c>
     </row>
     <row r="362" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
-        <v>2197</v>
+        <v>2202</v>
       </c>
       <c r="B362" t="s">
-        <v>2182</v>
+        <v>2201</v>
       </c>
       <c r="C362" t="s">
-        <v>2185</v>
+        <v>2203</v>
       </c>
       <c r="D362" t="s">
-        <v>2188</v>
+        <v>2204</v>
       </c>
       <c r="E362" t="s">
-        <v>2191</v>
+        <v>2205</v>
       </c>
       <c r="F362" t="s">
-        <v>2194</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="363" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
-        <v>2198</v>
+        <v>2192</v>
       </c>
       <c r="B363" t="s">
+        <v>2177</v>
+      </c>
+      <c r="C363" t="s">
+        <v>2180</v>
+      </c>
+      <c r="D363" t="s">
         <v>2183</v>
       </c>
-      <c r="C363" t="s">
+      <c r="E363" t="s">
         <v>2186</v>
       </c>
-      <c r="D363" t="s">
+      <c r="F363" t="s">
         <v>2189</v>
-      </c>
-      <c r="E363" t="s">
-        <v>2192</v>
-      </c>
-      <c r="F363" t="s">
-        <v>2195</v>
       </c>
     </row>
     <row r="364" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
-        <v>2199</v>
+        <v>2193</v>
       </c>
       <c r="B364" t="s">
+        <v>2178</v>
+      </c>
+      <c r="C364" t="s">
+        <v>2181</v>
+      </c>
+      <c r="D364" t="s">
         <v>2184</v>
       </c>
-      <c r="C364" t="s">
+      <c r="E364" t="s">
         <v>2187</v>
       </c>
-      <c r="D364" t="s">
+      <c r="F364" t="s">
         <v>2190</v>
-      </c>
-      <c r="E364" t="s">
-        <v>2193</v>
-      </c>
-      <c r="F364" t="s">
-        <v>2196</v>
       </c>
     </row>
     <row r="365" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
-        <v>2217</v>
+        <v>2194</v>
       </c>
       <c r="B365" t="s">
-        <v>2212</v>
+        <v>2179</v>
       </c>
       <c r="C365" t="s">
-        <v>2213</v>
+        <v>2182</v>
       </c>
       <c r="D365" t="s">
-        <v>2214</v>
+        <v>2185</v>
       </c>
       <c r="E365" t="s">
-        <v>2215</v>
+        <v>2188</v>
       </c>
       <c r="F365" t="s">
-        <v>2216</v>
+        <v>2191</v>
       </c>
     </row>
     <row r="366" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
-        <v>2218</v>
+        <v>2212</v>
       </c>
       <c r="B366" t="s">
-        <v>2219</v>
+        <v>2207</v>
       </c>
       <c r="C366" t="s">
-        <v>2220</v>
+        <v>2208</v>
       </c>
       <c r="D366" t="s">
-        <v>2221</v>
+        <v>2209</v>
       </c>
       <c r="E366" t="s">
-        <v>2222</v>
+        <v>2210</v>
       </c>
       <c r="F366" t="s">
-        <v>2223</v>
+        <v>2211</v>
       </c>
     </row>
     <row r="367" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
-        <v>2241</v>
+        <v>2213</v>
       </c>
       <c r="B367" t="s">
-        <v>2235</v>
+        <v>2214</v>
       </c>
       <c r="C367" t="s">
-        <v>2237</v>
+        <v>2215</v>
       </c>
       <c r="D367" t="s">
-        <v>2239</v>
+        <v>2216</v>
       </c>
       <c r="E367" t="s">
-        <v>2238</v>
+        <v>2217</v>
       </c>
       <c r="F367" t="s">
-        <v>2240</v>
+        <v>2218</v>
       </c>
     </row>
     <row r="368" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
-        <v>2224</v>
+        <v>2236</v>
       </c>
       <c r="B368" t="s">
-        <v>2225</v>
+        <v>2230</v>
       </c>
       <c r="C368" t="s">
-        <v>2236</v>
+        <v>2232</v>
       </c>
       <c r="D368" t="s">
-        <v>2226</v>
+        <v>2234</v>
       </c>
       <c r="E368" t="s">
-        <v>2227</v>
+        <v>2233</v>
       </c>
       <c r="F368" t="s">
-        <v>2228</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="369" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
-        <v>2234</v>
+        <v>2219</v>
       </c>
       <c r="B369" t="s">
-        <v>2229</v>
+        <v>2220</v>
       </c>
       <c r="C369" t="s">
         <v>2231</v>
       </c>
       <c r="D369" t="s">
-        <v>2230</v>
+        <v>2221</v>
       </c>
       <c r="E369" t="s">
-        <v>2232</v>
+        <v>2222</v>
       </c>
       <c r="F369" t="s">
-        <v>2233</v>
+        <v>2223</v>
       </c>
     </row>
     <row r="370" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
-        <v>2124</v>
+        <v>2229</v>
       </c>
       <c r="B370" t="s">
-        <v>2049</v>
+        <v>2224</v>
       </c>
       <c r="C370" t="s">
-        <v>2066</v>
+        <v>2226</v>
       </c>
       <c r="D370" t="s">
-        <v>2087</v>
+        <v>2225</v>
       </c>
       <c r="E370" t="s">
-        <v>2098</v>
+        <v>2227</v>
       </c>
       <c r="F370" t="s">
-        <v>2111</v>
+        <v>2228</v>
       </c>
     </row>
     <row r="371" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
-        <v>2162</v>
+        <v>2119</v>
       </c>
       <c r="B371" t="s">
-        <v>2142</v>
+        <v>2049</v>
       </c>
       <c r="C371" t="s">
-        <v>2149</v>
+        <v>2064</v>
       </c>
       <c r="D371" t="s">
-        <v>2150</v>
+        <v>2084</v>
       </c>
       <c r="E371" t="s">
-        <v>2154</v>
+        <v>2094</v>
       </c>
       <c r="F371" t="s">
-        <v>2158</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="372" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
-        <v>2163</v>
+        <v>2157</v>
       </c>
       <c r="B372" t="s">
-        <v>2143</v>
+        <v>2137</v>
       </c>
       <c r="C372" t="s">
-        <v>2146</v>
+        <v>2144</v>
       </c>
       <c r="D372" t="s">
-        <v>2151</v>
+        <v>2145</v>
       </c>
       <c r="E372" t="s">
-        <v>2155</v>
+        <v>2149</v>
       </c>
       <c r="F372" t="s">
-        <v>2159</v>
+        <v>2153</v>
       </c>
     </row>
     <row r="373" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
-        <v>2164</v>
+        <v>2158</v>
       </c>
       <c r="B373" t="s">
-        <v>2144</v>
+        <v>2138</v>
       </c>
       <c r="C373" t="s">
-        <v>2147</v>
+        <v>2141</v>
       </c>
       <c r="D373" t="s">
-        <v>2152</v>
+        <v>2146</v>
       </c>
       <c r="E373" t="s">
-        <v>2156</v>
+        <v>2150</v>
       </c>
       <c r="F373" t="s">
-        <v>2160</v>
+        <v>2154</v>
       </c>
     </row>
     <row r="374" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
-        <v>2165</v>
+        <v>2159</v>
       </c>
       <c r="B374" t="s">
-        <v>2145</v>
+        <v>2139</v>
       </c>
       <c r="C374" t="s">
-        <v>2148</v>
+        <v>2142</v>
       </c>
       <c r="D374" t="s">
-        <v>2153</v>
+        <v>2147</v>
       </c>
       <c r="E374" t="s">
-        <v>2157</v>
+        <v>2151</v>
       </c>
       <c r="F374" t="s">
-        <v>2161</v>
+        <v>2155</v>
       </c>
     </row>
     <row r="375" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
-        <v>2125</v>
+        <v>2160</v>
       </c>
       <c r="B375" t="s">
-        <v>2126</v>
+        <v>2140</v>
       </c>
       <c r="C375" t="s">
-        <v>2127</v>
+        <v>2143</v>
       </c>
       <c r="D375" t="s">
-        <v>2128</v>
+        <v>2148</v>
       </c>
       <c r="E375" t="s">
-        <v>2129</v>
+        <v>2152</v>
       </c>
       <c r="F375" t="s">
-        <v>2130</v>
+        <v>2156</v>
       </c>
     </row>
     <row r="376" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
-        <v>2201</v>
+        <v>2120</v>
       </c>
       <c r="B376" t="s">
-        <v>2200</v>
+        <v>2121</v>
       </c>
       <c r="C376" t="s">
-        <v>2202</v>
+        <v>2122</v>
       </c>
       <c r="D376" t="s">
-        <v>2203</v>
+        <v>2123</v>
       </c>
       <c r="E376" t="s">
-        <v>2204</v>
+        <v>2124</v>
       </c>
       <c r="F376" t="s">
-        <v>2205</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="377" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
+        <v>2196</v>
+      </c>
+      <c r="B377" t="s">
+        <v>2195</v>
+      </c>
+      <c r="C377" t="s">
+        <v>2197</v>
+      </c>
+      <c r="D377" t="s">
+        <v>2198</v>
+      </c>
+      <c r="E377" t="s">
+        <v>2199</v>
+      </c>
+      <c r="F377" t="s">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="378" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A378" t="s">
         <v>1503</v>
       </c>
-      <c r="B377" t="s">
+      <c r="B378" t="s">
         <v>1501</v>
       </c>
-      <c r="C377" t="s">
+      <c r="C378" t="s">
         <v>1502</v>
       </c>
-      <c r="D377" t="s">
+      <c r="D378" t="s">
         <v>1504</v>
       </c>
-      <c r="E377" t="s">
+      <c r="E378" t="s">
         <v>1505</v>
       </c>
-      <c r="F377" t="s">
+      <c r="F378" t="s">
         <v>1506</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update framework: new functions
</commit_message>
<xml_diff>
--- a/lang/words_dict.xlsx
+++ b/lang/words_dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Matlab Projects\Registration\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A2BFCC-AD9F-4210-922A-00FA0AA7FC46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E878A7-79C2-4F86-99DD-B268858925C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44040" yWindow="570" windowWidth="21600" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="1205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="1208">
   <si>
     <t>文件</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4198,12 +4198,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>您当前运行于服务器模式，独占模式可能造成MATLAB崩溃，继续？</t>
-  </si>
-  <si>
-    <t>You are currently running in server mode. Exclusive mode may cause MATLAB to crash. Continue?</t>
-  </si>
-  <si>
     <t>可用内存过小，独占模式启用失败</t>
   </si>
   <si>
@@ -4655,6 +4649,26 @@
   </si>
   <si>
     <t>LOW_MEMORY_WARNING</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>您当前运行于分布模式，独占模式可能造成MATLAB崩溃，继续？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>You are currently running in distributed mode. Exclusive mode may cause MATLAB to crash. Continue?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自动更新</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TEMPLATE_AUTO_UPDATE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Auto Update</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4989,10 +5003,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F403"/>
+  <dimension ref="A1:F404"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A391" workbookViewId="0">
-      <selection activeCell="B406" sqref="B406"/>
+    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
+      <selection activeCell="A279" sqref="A279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -5546,13 +5560,13 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="B50" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C50" t="s">
         <v>1195</v>
-      </c>
-      <c r="C50" t="s">
-        <v>1197</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
@@ -5568,13 +5582,13 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C52" t="s">
         <v>1093</v>
-      </c>
-      <c r="B52" t="s">
-        <v>1094</v>
-      </c>
-      <c r="C52" t="s">
-        <v>1095</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
@@ -5590,13 +5604,13 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="B54" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C54" t="s">
         <v>1096</v>
-      </c>
-      <c r="C54" t="s">
-        <v>1098</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -5799,13 +5813,13 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="B73" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="C73" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
@@ -6679,101 +6693,101 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="B153" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C153" t="s">
         <v>1143</v>
-      </c>
-      <c r="C153" t="s">
-        <v>1145</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="B154" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="C154" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="B155" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="C155" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="B156" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="C156" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="B157" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="C157" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B158" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C158" t="s">
         <v>1114</v>
-      </c>
-      <c r="B158" t="s">
-        <v>1111</v>
-      </c>
-      <c r="C158" t="s">
-        <v>1116</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B159" t="s">
+        <v>1110</v>
+      </c>
+      <c r="C159" t="s">
         <v>1115</v>
-      </c>
-      <c r="B159" t="s">
-        <v>1112</v>
-      </c>
-      <c r="C159" t="s">
-        <v>1117</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="B160" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="C160" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="B161" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="C161" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
@@ -6789,2652 +6803,2663 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>852</v>
+        <v>1206</v>
       </c>
       <c r="B163" t="s">
-        <v>122</v>
+        <v>1205</v>
       </c>
       <c r="C163" t="s">
-        <v>359</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>558</v>
+        <v>852</v>
       </c>
       <c r="B164" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C164" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B165" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C165" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B166" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C166" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>778</v>
+        <v>560</v>
       </c>
       <c r="B167" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C167" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B168" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C168" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>770</v>
+        <v>779</v>
       </c>
       <c r="B169" t="s">
-        <v>14</v>
+        <v>127</v>
       </c>
       <c r="C169" t="s">
-        <v>774</v>
+        <v>364</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="B170" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C170" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="B171" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C171" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="B172" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C172" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>800</v>
+        <v>773</v>
       </c>
       <c r="B173" t="s">
-        <v>130</v>
+        <v>11</v>
       </c>
       <c r="C173" t="s">
-        <v>367</v>
+        <v>777</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>1122</v>
+        <v>800</v>
       </c>
       <c r="B174" t="s">
-        <v>1120</v>
+        <v>130</v>
       </c>
       <c r="C174" t="s">
-        <v>1121</v>
+        <v>367</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>858</v>
+        <v>1120</v>
       </c>
       <c r="B175" t="s">
-        <v>131</v>
+        <v>1118</v>
       </c>
       <c r="C175" t="s">
-        <v>368</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="B176" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C176" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>1102</v>
+        <v>860</v>
       </c>
       <c r="B177" t="s">
-        <v>1099</v>
+        <v>132</v>
       </c>
       <c r="C177" t="s">
-        <v>1105</v>
+        <v>369</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B178" t="s">
+        <v>1097</v>
+      </c>
+      <c r="C178" t="s">
         <v>1103</v>
-      </c>
-      <c r="B178" t="s">
-        <v>1100</v>
-      </c>
-      <c r="C178" t="s">
-        <v>1106</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B179" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C179" t="s">
         <v>1104</v>
-      </c>
-      <c r="B179" t="s">
-        <v>1101</v>
-      </c>
-      <c r="C179" t="s">
-        <v>1107</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>1110</v>
+        <v>1102</v>
       </c>
       <c r="B180" t="s">
-        <v>1108</v>
+        <v>1099</v>
       </c>
       <c r="C180" t="s">
-        <v>1109</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>562</v>
+        <v>1108</v>
       </c>
       <c r="B181" t="s">
-        <v>133</v>
+        <v>1106</v>
       </c>
       <c r="C181" t="s">
-        <v>370</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>1080</v>
+        <v>562</v>
       </c>
       <c r="B182" t="s">
-        <v>1079</v>
+        <v>133</v>
       </c>
       <c r="C182" t="s">
-        <v>1081</v>
+        <v>370</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>563</v>
+        <v>1080</v>
       </c>
       <c r="B183" t="s">
-        <v>134</v>
+        <v>1079</v>
       </c>
       <c r="C183" t="s">
-        <v>371</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>1123</v>
+        <v>563</v>
       </c>
       <c r="B184" t="s">
-        <v>1124</v>
+        <v>134</v>
       </c>
       <c r="C184" t="s">
-        <v>1125</v>
+        <v>371</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>1020</v>
+        <v>1121</v>
       </c>
       <c r="B185" t="s">
-        <v>135</v>
+        <v>1122</v>
       </c>
       <c r="C185" t="s">
-        <v>372</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>564</v>
+        <v>1020</v>
       </c>
       <c r="B186" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C186" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B187" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C187" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>907</v>
+        <v>565</v>
       </c>
       <c r="B188" t="s">
-        <v>908</v>
+        <v>137</v>
       </c>
       <c r="C188" t="s">
-        <v>909</v>
+        <v>374</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>1182</v>
+        <v>907</v>
       </c>
       <c r="B189" t="s">
-        <v>1178</v>
+        <v>908</v>
       </c>
       <c r="C189" t="s">
-        <v>1180</v>
+        <v>909</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>1183</v>
+        <v>1180</v>
       </c>
       <c r="B190" t="s">
-        <v>1179</v>
+        <v>1176</v>
       </c>
       <c r="C190" t="s">
-        <v>1181</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>861</v>
+        <v>1181</v>
       </c>
       <c r="B191" t="s">
-        <v>138</v>
+        <v>1177</v>
       </c>
       <c r="C191" t="s">
-        <v>375</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>566</v>
+        <v>861</v>
       </c>
       <c r="B192" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C192" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>821</v>
+        <v>566</v>
       </c>
       <c r="B193" t="s">
-        <v>807</v>
+        <v>139</v>
       </c>
       <c r="C193" t="s">
-        <v>822</v>
+        <v>376</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>855</v>
+        <v>821</v>
       </c>
       <c r="B194" t="s">
-        <v>129</v>
+        <v>807</v>
       </c>
       <c r="C194" t="s">
-        <v>366</v>
+        <v>822</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B195" t="s">
-        <v>764</v>
+        <v>129</v>
       </c>
       <c r="C195" t="s">
-        <v>765</v>
+        <v>366</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>825</v>
+        <v>856</v>
       </c>
       <c r="B196" t="s">
-        <v>808</v>
+        <v>764</v>
       </c>
       <c r="C196" t="s">
-        <v>823</v>
+        <v>765</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B197" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="C197" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="B198" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="C198" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="B199" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C199" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="B200" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="C200" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B201" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C201" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="B202" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="C202" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="B203" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C203" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="B204" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C204" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="B205" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C205" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="B206" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="C206" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="B207" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C207" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B208" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C208" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>561</v>
+        <v>847</v>
       </c>
       <c r="B209" t="s">
-        <v>128</v>
+        <v>820</v>
       </c>
       <c r="C209" t="s">
-        <v>365</v>
+        <v>848</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="B210" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C210" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B211" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C211" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B212" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C212" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B213" t="s">
-        <v>1161</v>
+        <v>142</v>
       </c>
       <c r="C213" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B214" t="s">
-        <v>143</v>
+        <v>1159</v>
       </c>
       <c r="C214" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B215" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C215" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B216" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C216" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>859</v>
+        <v>573</v>
       </c>
       <c r="B217" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C217" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>854</v>
+        <v>859</v>
       </c>
       <c r="B218" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C218" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>1166</v>
+        <v>854</v>
       </c>
       <c r="B219" t="s">
-        <v>1162</v>
+        <v>147</v>
       </c>
       <c r="C219" t="s">
-        <v>1165</v>
+        <v>385</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>1174</v>
+        <v>1164</v>
       </c>
       <c r="B220" t="s">
-        <v>1171</v>
+        <v>1160</v>
       </c>
       <c r="C220" t="s">
-        <v>1175</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>1184</v>
+        <v>1172</v>
       </c>
       <c r="B221" t="s">
-        <v>1172</v>
+        <v>1169</v>
       </c>
       <c r="C221" t="s">
-        <v>1176</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>1185</v>
+        <v>1182</v>
       </c>
       <c r="B222" t="s">
-        <v>1173</v>
+        <v>1170</v>
       </c>
       <c r="C222" t="s">
-        <v>1177</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>1168</v>
+        <v>1183</v>
       </c>
       <c r="B223" t="s">
-        <v>1163</v>
+        <v>1171</v>
       </c>
       <c r="C223" t="s">
-        <v>1167</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>1170</v>
+        <v>1166</v>
       </c>
       <c r="B224" t="s">
-        <v>1164</v>
+        <v>1161</v>
       </c>
       <c r="C224" t="s">
-        <v>1169</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>857</v>
+        <v>1168</v>
       </c>
       <c r="B225" t="s">
-        <v>148</v>
+        <v>1162</v>
       </c>
       <c r="C225" t="s">
-        <v>386</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>1141</v>
+        <v>857</v>
       </c>
       <c r="B226" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C226" t="s">
-        <v>1142</v>
+        <v>386</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>862</v>
+        <v>1139</v>
       </c>
       <c r="B227" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C227" t="s">
-        <v>387</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>1189</v>
+        <v>862</v>
       </c>
       <c r="B228" t="s">
-        <v>1186</v>
+        <v>150</v>
       </c>
       <c r="C228" t="s">
-        <v>1192</v>
+        <v>387</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
+        <v>1187</v>
+      </c>
+      <c r="B229" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C229" t="s">
         <v>1190</v>
-      </c>
-      <c r="B229" t="s">
-        <v>1187</v>
-      </c>
-      <c r="C229" t="s">
-        <v>1193</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B230" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C230" t="s">
         <v>1191</v>
-      </c>
-      <c r="B230" t="s">
-        <v>1188</v>
-      </c>
-      <c r="C230" t="s">
-        <v>1194</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>1021</v>
+        <v>1189</v>
       </c>
       <c r="B231" t="s">
-        <v>151</v>
+        <v>1186</v>
       </c>
       <c r="C231" t="s">
-        <v>388</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>574</v>
+        <v>1021</v>
       </c>
       <c r="B232" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C232" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B233" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C233" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B234" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C234" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B235" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C235" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B236" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C236" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B237" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C237" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B238" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C238" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B239" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C239" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B240" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C240" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B241" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C241" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B242" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C242" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B243" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C243" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B244" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C244" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B245" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C245" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B246" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C246" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B247" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C247" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>604</v>
+        <v>589</v>
       </c>
       <c r="B248" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C248" t="s">
-        <v>478</v>
+        <v>404</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>590</v>
+        <v>604</v>
       </c>
       <c r="B249" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C249" t="s">
-        <v>405</v>
+        <v>478</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B250" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C250" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B251" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C251" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B252" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C252" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B253" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C253" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B254" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C254" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B255" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C255" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B256" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C256" t="s">
-        <v>605</v>
+        <v>411</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B257" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C257" t="s">
-        <v>412</v>
+        <v>605</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>693</v>
+        <v>598</v>
       </c>
       <c r="B258" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C258" t="s">
-        <v>448</v>
+        <v>412</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
-        <v>606</v>
+        <v>693</v>
       </c>
       <c r="B259" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C259" t="s">
-        <v>413</v>
+        <v>448</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
-        <v>910</v>
+        <v>606</v>
       </c>
       <c r="B260" t="s">
-        <v>911</v>
+        <v>179</v>
       </c>
       <c r="C260" t="s">
-        <v>912</v>
+        <v>413</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
-        <v>607</v>
+        <v>910</v>
       </c>
       <c r="B261" t="s">
-        <v>180</v>
+        <v>911</v>
       </c>
       <c r="C261" t="s">
-        <v>449</v>
+        <v>912</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B262" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C262" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B263" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C263" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
-        <v>780</v>
+        <v>609</v>
       </c>
       <c r="B264" t="s">
-        <v>781</v>
+        <v>182</v>
       </c>
       <c r="C264" t="s">
-        <v>782</v>
+        <v>451</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="B265" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="C265" t="s">
-        <v>788</v>
+        <v>782</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="B266" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="C266" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
-        <v>790</v>
+        <v>785</v>
       </c>
       <c r="B267" t="s">
-        <v>792</v>
+        <v>786</v>
       </c>
       <c r="C267" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="B268" t="s">
-        <v>789</v>
+        <v>792</v>
       </c>
       <c r="C268" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="B269" t="s">
-        <v>796</v>
+        <v>789</v>
       </c>
       <c r="C269" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="B270" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="C270" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
-        <v>610</v>
+        <v>797</v>
       </c>
       <c r="B271" t="s">
-        <v>183</v>
+        <v>798</v>
       </c>
       <c r="C271" t="s">
-        <v>414</v>
+        <v>799</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B272" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C272" t="s">
-        <v>452</v>
+        <v>414</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B273" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C273" t="s">
-        <v>415</v>
+        <v>452</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B274" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C274" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
-        <v>1202</v>
+        <v>613</v>
       </c>
       <c r="B275" t="s">
-        <v>1201</v>
+        <v>186</v>
       </c>
       <c r="C275" t="s">
-        <v>1203</v>
+        <v>416</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
-        <v>615</v>
+        <v>1200</v>
       </c>
       <c r="B276" t="s">
-        <v>188</v>
+        <v>1199</v>
       </c>
       <c r="C276" t="s">
-        <v>417</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
-        <v>806</v>
+        <v>615</v>
       </c>
       <c r="B277" t="s">
-        <v>804</v>
+        <v>188</v>
       </c>
       <c r="C277" t="s">
-        <v>805</v>
+        <v>417</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
-        <v>616</v>
+        <v>806</v>
       </c>
       <c r="B278" t="s">
-        <v>726</v>
+        <v>804</v>
       </c>
       <c r="C278" t="s">
-        <v>727</v>
+        <v>805</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B279" t="s">
-        <v>189</v>
+        <v>726</v>
       </c>
       <c r="C279" t="s">
-        <v>418</v>
+        <v>727</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B280" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C280" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B281" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C281" t="s">
-        <v>471</v>
+        <v>419</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B282" t="s">
-        <v>724</v>
+        <v>191</v>
       </c>
       <c r="C282" t="s">
-        <v>725</v>
+        <v>471</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B283" t="s">
-        <v>192</v>
+        <v>724</v>
       </c>
       <c r="C283" t="s">
-        <v>420</v>
+        <v>725</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B284" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C284" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B285" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C285" t="s">
-        <v>453</v>
+        <v>421</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B286" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C286" t="s">
-        <v>422</v>
+        <v>453</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B287" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="C287" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B288" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C288" t="s">
-        <v>479</v>
+        <v>423</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B289" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C289" t="s">
-        <v>424</v>
+        <v>479</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B290" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C290" t="s">
-        <v>480</v>
+        <v>424</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B291" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="C291" t="s">
-        <v>425</v>
+        <v>480</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B292" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C292" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B293" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C293" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B294" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C294" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B295" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C295" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
-        <v>729</v>
+        <v>633</v>
       </c>
       <c r="B296" t="s">
-        <v>728</v>
+        <v>200</v>
       </c>
       <c r="C296" t="s">
-        <v>730</v>
+        <v>429</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
-        <v>634</v>
+        <v>729</v>
       </c>
       <c r="B297" t="s">
-        <v>201</v>
+        <v>728</v>
       </c>
       <c r="C297" t="s">
-        <v>455</v>
+        <v>730</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B298" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C298" t="s">
-        <v>430</v>
+        <v>455</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B299" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C299" t="s">
-        <v>469</v>
+        <v>430</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B300" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C300" t="s">
-        <v>874</v>
+        <v>469</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
-        <v>872</v>
+        <v>637</v>
       </c>
       <c r="B301" t="s">
-        <v>873</v>
+        <v>204</v>
       </c>
       <c r="C301" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
-        <v>638</v>
+        <v>872</v>
       </c>
       <c r="B302" t="s">
-        <v>205</v>
+        <v>873</v>
       </c>
       <c r="C302" t="s">
-        <v>431</v>
+        <v>875</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B303" t="s">
-        <v>24</v>
+        <v>205</v>
       </c>
       <c r="C303" t="s">
-        <v>468</v>
+        <v>431</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B304" t="s">
-        <v>206</v>
+        <v>24</v>
       </c>
       <c r="C304" t="s">
-        <v>432</v>
+        <v>468</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
-        <v>720</v>
+        <v>640</v>
       </c>
       <c r="B305" t="s">
-        <v>719</v>
+        <v>206</v>
       </c>
       <c r="C305" t="s">
-        <v>721</v>
+        <v>432</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
-        <v>641</v>
+        <v>720</v>
       </c>
       <c r="B306" t="s">
-        <v>207</v>
+        <v>719</v>
       </c>
       <c r="C306" t="s">
-        <v>470</v>
+        <v>721</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B307" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C307" t="s">
-        <v>454</v>
+        <v>470</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
-        <v>671</v>
+        <v>642</v>
       </c>
       <c r="B308" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C308" t="s">
-        <v>433</v>
+        <v>454</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
-        <v>644</v>
+        <v>671</v>
       </c>
       <c r="B309" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C309" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B310" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C310" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="B311" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C311" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="B312" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C312" t="s">
-        <v>457</v>
+        <v>436</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B313" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C313" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="B314" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C314" t="s">
-        <v>437</v>
+        <v>458</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B315" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C315" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B316" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C316" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B317" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C317" t="s">
-        <v>677</v>
+        <v>439</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
-        <v>722</v>
+        <v>654</v>
       </c>
       <c r="B318" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C318" t="s">
-        <v>440</v>
+        <v>677</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
-        <v>655</v>
+        <v>722</v>
       </c>
       <c r="B319" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C319" t="s">
-        <v>459</v>
+        <v>440</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
-        <v>651</v>
+        <v>655</v>
       </c>
       <c r="B320" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C320" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
-        <v>733</v>
+        <v>651</v>
       </c>
       <c r="B321" t="s">
-        <v>731</v>
+        <v>225</v>
       </c>
       <c r="C321" t="s">
-        <v>732</v>
+        <v>460</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
-        <v>643</v>
+        <v>733</v>
       </c>
       <c r="B322" t="s">
-        <v>226</v>
+        <v>731</v>
       </c>
       <c r="C322" t="s">
-        <v>461</v>
+        <v>732</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
-        <v>656</v>
+        <v>643</v>
       </c>
       <c r="B323" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C323" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B324" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C324" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B325" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C325" t="s">
-        <v>659</v>
+        <v>463</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="B326" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C326" t="s">
-        <v>441</v>
+        <v>659</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="B327" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C327" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B328" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C328" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
-        <v>734</v>
+        <v>661</v>
       </c>
       <c r="B329" t="s">
-        <v>736</v>
+        <v>232</v>
       </c>
       <c r="C329" t="s">
-        <v>735</v>
+        <v>443</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
-        <v>663</v>
+        <v>734</v>
       </c>
       <c r="B330" t="s">
-        <v>233</v>
+        <v>736</v>
       </c>
       <c r="C330" t="s">
-        <v>464</v>
+        <v>735</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B331" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C331" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B332" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C332" t="s">
-        <v>444</v>
+        <v>465</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B333" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C333" t="s">
-        <v>466</v>
+        <v>444</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B334" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C334" t="s">
-        <v>445</v>
+        <v>466</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
-        <v>880</v>
+        <v>667</v>
       </c>
       <c r="B335" t="s">
-        <v>879</v>
+        <v>237</v>
       </c>
       <c r="C335" t="s">
-        <v>881</v>
+        <v>445</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
-        <v>668</v>
+        <v>880</v>
       </c>
       <c r="B336" t="s">
-        <v>238</v>
+        <v>879</v>
       </c>
       <c r="C336" t="s">
-        <v>446</v>
+        <v>881</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
-        <v>649</v>
+        <v>668</v>
       </c>
       <c r="B337" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C337" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A338" t="s">
-        <v>669</v>
+        <v>649</v>
       </c>
       <c r="B338" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C338" t="s">
-        <v>885</v>
+        <v>447</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A339" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B339" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C339" t="s">
-        <v>467</v>
+        <v>885</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
-        <v>747</v>
+        <v>670</v>
       </c>
       <c r="B340" t="s">
-        <v>745</v>
+        <v>241</v>
       </c>
       <c r="C340" t="s">
-        <v>746</v>
+        <v>467</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="B341" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="C341" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A342" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="B342" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="C342" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A343" t="s">
-        <v>1127</v>
+        <v>753</v>
       </c>
       <c r="B343" t="s">
-        <v>1131</v>
+        <v>751</v>
       </c>
       <c r="C343" t="s">
-        <v>1132</v>
+        <v>752</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A344" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B344" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C344" t="s">
         <v>1130</v>
-      </c>
-      <c r="B344" t="s">
-        <v>1133</v>
-      </c>
-      <c r="C344" t="s">
-        <v>1134</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A345" t="s">
-        <v>1126</v>
+        <v>1128</v>
       </c>
       <c r="B345" t="s">
-        <v>1135</v>
+        <v>1131</v>
       </c>
       <c r="C345" t="s">
-        <v>1136</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A346" t="s">
-        <v>1128</v>
+        <v>1124</v>
       </c>
       <c r="B346" t="s">
-        <v>1137</v>
+        <v>1133</v>
       </c>
       <c r="C346" t="s">
-        <v>1138</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
-        <v>1129</v>
+        <v>1126</v>
       </c>
       <c r="B347" t="s">
-        <v>1139</v>
+        <v>1135</v>
       </c>
       <c r="C347" t="s">
-        <v>1140</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A348" t="s">
-        <v>757</v>
+        <v>1127</v>
       </c>
       <c r="B348" t="s">
-        <v>754</v>
+        <v>1137</v>
       </c>
       <c r="C348" t="s">
-        <v>756</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="B349" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C349" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="B350" t="s">
-        <v>761</v>
+        <v>755</v>
       </c>
       <c r="C350" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A351" t="s">
-        <v>697</v>
+        <v>762</v>
       </c>
       <c r="B351" t="s">
-        <v>681</v>
+        <v>761</v>
       </c>
       <c r="C351" t="s">
-        <v>710</v>
+        <v>760</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A352" t="s">
-        <v>711</v>
+        <v>697</v>
       </c>
       <c r="B352" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C352" t="s">
-        <v>706</v>
+        <v>710</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B353" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C353" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
-        <v>698</v>
+        <v>712</v>
       </c>
       <c r="B354" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C354" t="s">
-        <v>718</v>
+        <v>707</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B355" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="C355" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B356" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C356" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B357" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C357" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B358" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C358" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B359" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C359" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B360" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C360" t="s">
-        <v>708</v>
+        <v>713</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B361" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C361" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
-        <v>803</v>
+        <v>705</v>
       </c>
       <c r="B362" t="s">
-        <v>801</v>
+        <v>691</v>
       </c>
       <c r="C362" t="s">
-        <v>802</v>
+        <v>709</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
-        <v>850</v>
+        <v>803</v>
       </c>
       <c r="B363" t="s">
-        <v>849</v>
+        <v>801</v>
       </c>
       <c r="C363" t="s">
-        <v>851</v>
+        <v>802</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
-        <v>933</v>
+        <v>850</v>
       </c>
       <c r="B364" t="s">
-        <v>929</v>
+        <v>849</v>
       </c>
       <c r="C364" t="s">
-        <v>931</v>
+        <v>851</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B365" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="C365" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
-        <v>951</v>
+        <v>934</v>
       </c>
       <c r="B366" t="s">
-        <v>950</v>
+        <v>930</v>
       </c>
       <c r="C366" t="s">
-        <v>952</v>
+        <v>932</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
-        <v>985</v>
+        <v>951</v>
       </c>
       <c r="B367" t="s">
-        <v>960</v>
+        <v>950</v>
       </c>
       <c r="C367" t="s">
-        <v>972</v>
+        <v>952</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="B368" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="C368" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A369" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="B369" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="C369" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A370" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="B370" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="C370" t="s">
-        <v>978</v>
+        <v>974</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A371" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="B371" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="C371" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A372" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="B372" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="C372" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A373" t="s">
-        <v>1024</v>
+        <v>989</v>
       </c>
       <c r="B373" t="s">
-        <v>1023</v>
+        <v>966</v>
       </c>
       <c r="C373" t="s">
-        <v>1025</v>
+        <v>980</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A374" t="s">
-        <v>990</v>
+        <v>1024</v>
       </c>
       <c r="B374" t="s">
-        <v>967</v>
+        <v>1023</v>
       </c>
       <c r="C374" t="s">
-        <v>981</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A375" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B375" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="C375" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A376" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B376" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="C376" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A377" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="B377" t="s">
-        <v>975</v>
+        <v>969</v>
       </c>
       <c r="C377" t="s">
-        <v>976</v>
+        <v>983</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A378" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B378" t="s">
-        <v>1062</v>
+        <v>975</v>
       </c>
       <c r="C378" t="s">
-        <v>1066</v>
+        <v>976</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A379" t="s">
-        <v>1065</v>
+        <v>994</v>
       </c>
       <c r="B379" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C379" t="s">
-        <v>1064</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A380" t="s">
-        <v>995</v>
+        <v>1065</v>
       </c>
       <c r="B380" t="s">
-        <v>970</v>
+        <v>1063</v>
       </c>
       <c r="C380" t="s">
-        <v>971</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
-        <v>1027</v>
+        <v>995</v>
       </c>
       <c r="B381" t="s">
-        <v>1026</v>
+        <v>970</v>
       </c>
       <c r="C381" t="s">
-        <v>1028</v>
+        <v>971</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A382" t="s">
-        <v>1042</v>
+        <v>1027</v>
       </c>
       <c r="B382" t="s">
-        <v>1041</v>
+        <v>1026</v>
       </c>
       <c r="C382" t="s">
-        <v>1043</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A383" t="s">
-        <v>1035</v>
+        <v>1042</v>
       </c>
       <c r="B383" t="s">
-        <v>1029</v>
+        <v>1041</v>
       </c>
       <c r="C383" t="s">
-        <v>1032</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A384" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B384" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="C384" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A385" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="B385" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="C385" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A386" t="s">
-        <v>1046</v>
+        <v>1037</v>
       </c>
       <c r="B386" t="s">
-        <v>1044</v>
+        <v>1031</v>
       </c>
       <c r="C386" t="s">
-        <v>1045</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A387" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="B387" t="s">
-        <v>1048</v>
+        <v>1044</v>
       </c>
       <c r="C387" t="s">
-        <v>1049</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A388" t="s">
-        <v>1058</v>
+        <v>1047</v>
       </c>
       <c r="B388" t="s">
-        <v>1055</v>
+        <v>1048</v>
       </c>
       <c r="C388" t="s">
-        <v>1057</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A389" t="s">
-        <v>1050</v>
+        <v>1058</v>
       </c>
       <c r="B389" t="s">
-        <v>1051</v>
+        <v>1055</v>
       </c>
       <c r="C389" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A390" t="s">
-        <v>1054</v>
+        <v>1050</v>
       </c>
       <c r="B390" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="C390" t="s">
-        <v>1053</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A391" t="s">
-        <v>996</v>
+        <v>1054</v>
       </c>
       <c r="B391" t="s">
-        <v>962</v>
+        <v>1052</v>
       </c>
       <c r="C391" t="s">
-        <v>977</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A392" t="s">
-        <v>1016</v>
+        <v>996</v>
       </c>
       <c r="B392" t="s">
-        <v>1008</v>
+        <v>962</v>
       </c>
       <c r="C392" t="s">
-        <v>1015</v>
+        <v>977</v>
       </c>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A393" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B393" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="C393" t="s">
-        <v>1012</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A394" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B394" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="C394" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A395" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B395" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="C395" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A396" t="s">
-        <v>997</v>
+        <v>1019</v>
       </c>
       <c r="B396" t="s">
-        <v>998</v>
+        <v>1011</v>
       </c>
       <c r="C396" t="s">
-        <v>999</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A397" t="s">
-        <v>1039</v>
+        <v>997</v>
       </c>
       <c r="B397" t="s">
-        <v>1038</v>
+        <v>998</v>
       </c>
       <c r="C397" t="s">
-        <v>1040</v>
+        <v>999</v>
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A398" t="s">
-        <v>1073</v>
+        <v>1039</v>
       </c>
       <c r="B398" t="s">
-        <v>1067</v>
+        <v>1038</v>
       </c>
       <c r="C398" t="s">
-        <v>1071</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A399" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="B399" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
       <c r="C399" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A400" t="s">
-        <v>1078</v>
+        <v>1074</v>
       </c>
       <c r="B400" t="s">
-        <v>1075</v>
+        <v>1070</v>
       </c>
       <c r="C400" t="s">
-        <v>1076</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A401" t="s">
-        <v>1088</v>
+        <v>1078</v>
       </c>
       <c r="B401" t="s">
-        <v>1089</v>
+        <v>1075</v>
       </c>
       <c r="C401" t="s">
-        <v>1090</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A402" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B402" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C402" t="s">
         <v>1204</v>
-      </c>
-      <c r="B402" t="s">
-        <v>1091</v>
-      </c>
-      <c r="C402" t="s">
-        <v>1092</v>
       </c>
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A403" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B403" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C403" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="404" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A404" t="s">
         <v>696</v>
       </c>
-      <c r="B403" t="s">
+      <c r="B404" t="s">
         <v>694</v>
       </c>
-      <c r="C403" t="s">
+      <c r="C404" t="s">
         <v>695</v>
       </c>
     </row>

</xml_diff>